<commit_message>
- changed col_id to ID
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_GINI_P1.xlsx
+++ b/rmonize/data_dictionary/DD_GINI_P1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{D573B252-DF39-40CE-801D-A214E9FF7CB3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBF8566-83AC-446A-97EF-862086C728ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
   </bookViews>
@@ -40,9 +40,6 @@
     <t>valueType</t>
   </si>
   <si>
-    <t>col_id</t>
-  </si>
-  <si>
     <t>ID of the participant</t>
   </si>
   <si>
@@ -630,6 +627,9 @@
   </si>
   <si>
     <t>yes, less often</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -1050,7 +1050,7 @@
   <dimension ref="A1:D90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1079,13 +1079,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1093,13 +1093,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>8</v>
-      </c>
       <c r="D3" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1107,13 +1107,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>10</v>
-      </c>
       <c r="D4" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1121,13 +1121,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="D5" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1135,13 +1135,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>14</v>
-      </c>
       <c r="D6" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1149,13 +1149,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1163,13 +1163,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="D8" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1177,13 +1177,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>21</v>
-      </c>
       <c r="D9" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1191,13 +1191,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
         <v>22</v>
       </c>
-      <c r="C10" t="s">
-        <v>23</v>
-      </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1205,13 +1205,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
         <v>24</v>
       </c>
-      <c r="C11" t="s">
-        <v>25</v>
-      </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1219,13 +1219,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
         <v>26</v>
       </c>
-      <c r="C12" t="s">
-        <v>27</v>
-      </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1233,13 +1233,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
         <v>28</v>
       </c>
-      <c r="C13" t="s">
-        <v>29</v>
-      </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1247,13 +1247,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
         <v>30</v>
       </c>
-      <c r="C14" t="s">
-        <v>31</v>
-      </c>
       <c r="D14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1261,13 +1261,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
         <v>32</v>
       </c>
-      <c r="C15" t="s">
-        <v>33</v>
-      </c>
       <c r="D15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1275,13 +1275,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s">
         <v>34</v>
       </c>
-      <c r="C16" t="s">
-        <v>35</v>
-      </c>
       <c r="D16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1289,13 +1289,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" t="s">
         <v>36</v>
       </c>
-      <c r="C17" t="s">
-        <v>37</v>
-      </c>
       <c r="D17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1303,13 +1303,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" t="s">
         <v>38</v>
       </c>
-      <c r="C18" t="s">
-        <v>39</v>
-      </c>
       <c r="D18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1317,13 +1317,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" t="s">
         <v>40</v>
       </c>
-      <c r="C19" t="s">
-        <v>41</v>
-      </c>
       <c r="D19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1331,13 +1331,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" t="s">
         <v>42</v>
       </c>
-      <c r="C20" t="s">
-        <v>43</v>
-      </c>
       <c r="D20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1345,13 +1345,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" t="s">
         <v>44</v>
       </c>
-      <c r="C21" t="s">
-        <v>45</v>
-      </c>
       <c r="D21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1359,13 +1359,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" t="s">
         <v>46</v>
       </c>
-      <c r="C22" t="s">
-        <v>47</v>
-      </c>
       <c r="D22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1373,13 +1373,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" t="s">
         <v>48</v>
       </c>
-      <c r="C23" t="s">
-        <v>49</v>
-      </c>
       <c r="D23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1387,13 +1387,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" t="s">
         <v>50</v>
       </c>
-      <c r="C24" t="s">
-        <v>51</v>
-      </c>
       <c r="D24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1401,13 +1401,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" t="s">
         <v>52</v>
       </c>
-      <c r="C25" t="s">
-        <v>53</v>
-      </c>
       <c r="D25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1415,13 +1415,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" t="s">
         <v>54</v>
       </c>
-      <c r="C26" t="s">
-        <v>55</v>
-      </c>
       <c r="D26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1429,13 +1429,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="D27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1443,13 +1443,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" t="s">
         <v>58</v>
       </c>
-      <c r="C28" t="s">
-        <v>59</v>
-      </c>
       <c r="D28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1457,13 +1457,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" t="s">
         <v>60</v>
       </c>
-      <c r="C29" t="s">
-        <v>61</v>
-      </c>
       <c r="D29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1471,13 +1471,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" t="s">
         <v>62</v>
       </c>
-      <c r="C30" t="s">
-        <v>63</v>
-      </c>
       <c r="D30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1485,13 +1485,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" t="s">
         <v>64</v>
       </c>
-      <c r="C31" t="s">
-        <v>65</v>
-      </c>
       <c r="D31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1499,13 +1499,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" t="s">
         <v>66</v>
       </c>
-      <c r="C32" t="s">
-        <v>67</v>
-      </c>
       <c r="D32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1513,13 +1513,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" t="s">
         <v>68</v>
       </c>
-      <c r="C33" t="s">
-        <v>69</v>
-      </c>
       <c r="D33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1527,13 +1527,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" t="s">
         <v>70</v>
       </c>
-      <c r="C34" t="s">
-        <v>71</v>
-      </c>
       <c r="D34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1541,13 +1541,13 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" t="s">
         <v>72</v>
       </c>
-      <c r="C35" t="s">
-        <v>73</v>
-      </c>
       <c r="D35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1555,13 +1555,13 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" t="s">
         <v>74</v>
       </c>
-      <c r="C36" t="s">
-        <v>75</v>
-      </c>
       <c r="D36" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1569,13 +1569,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" t="s">
         <v>76</v>
       </c>
-      <c r="C37" t="s">
-        <v>77</v>
-      </c>
       <c r="D37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1583,13 +1583,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38" t="s">
         <v>78</v>
       </c>
-      <c r="C38" t="s">
-        <v>79</v>
-      </c>
       <c r="D38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1597,13 +1597,13 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" t="s">
         <v>80</v>
       </c>
-      <c r="C39" t="s">
-        <v>81</v>
-      </c>
       <c r="D39" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1611,13 +1611,13 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" t="s">
         <v>82</v>
       </c>
-      <c r="C40" t="s">
-        <v>83</v>
-      </c>
       <c r="D40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1625,13 +1625,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C41" s="13" t="s">
-        <v>85</v>
-      </c>
       <c r="D41" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1639,13 +1639,13 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" t="s">
         <v>86</v>
       </c>
-      <c r="C42" t="s">
-        <v>87</v>
-      </c>
       <c r="D42" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1653,13 +1653,13 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43" t="s">
         <v>88</v>
       </c>
-      <c r="C43" t="s">
-        <v>89</v>
-      </c>
       <c r="D43" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1667,13 +1667,13 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" t="s">
         <v>90</v>
       </c>
-      <c r="C44" t="s">
-        <v>91</v>
-      </c>
       <c r="D44" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1681,13 +1681,13 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45" t="s">
         <v>92</v>
       </c>
-      <c r="C45" t="s">
-        <v>93</v>
-      </c>
       <c r="D45" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1695,13 +1695,13 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
+        <v>93</v>
+      </c>
+      <c r="C46" t="s">
         <v>94</v>
       </c>
-      <c r="C46" t="s">
-        <v>95</v>
-      </c>
       <c r="D46" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1709,13 +1709,13 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
+        <v>95</v>
+      </c>
+      <c r="C47" t="s">
         <v>96</v>
       </c>
-      <c r="C47" t="s">
-        <v>97</v>
-      </c>
       <c r="D47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1723,13 +1723,13 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" t="s">
         <v>98</v>
       </c>
-      <c r="C48" t="s">
-        <v>99</v>
-      </c>
       <c r="D48" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1737,13 +1737,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C49" t="s">
         <v>100</v>
       </c>
-      <c r="C49" t="s">
-        <v>101</v>
-      </c>
       <c r="D49" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1751,13 +1751,13 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C50" t="s">
         <v>102</v>
       </c>
-      <c r="C50" t="s">
-        <v>103</v>
-      </c>
       <c r="D50" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1765,13 +1765,13 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
+        <v>103</v>
+      </c>
+      <c r="C51" t="s">
         <v>104</v>
       </c>
-      <c r="C51" t="s">
-        <v>105</v>
-      </c>
       <c r="D51" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1779,13 +1779,13 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
+        <v>105</v>
+      </c>
+      <c r="C52" t="s">
         <v>106</v>
       </c>
-      <c r="C52" t="s">
-        <v>107</v>
-      </c>
       <c r="D52" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1793,13 +1793,13 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
+        <v>107</v>
+      </c>
+      <c r="C53" t="s">
         <v>108</v>
       </c>
-      <c r="C53" t="s">
-        <v>109</v>
-      </c>
       <c r="D53" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1807,13 +1807,13 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
+        <v>109</v>
+      </c>
+      <c r="C54" t="s">
         <v>110</v>
       </c>
-      <c r="C54" t="s">
-        <v>111</v>
-      </c>
       <c r="D54" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1821,13 +1821,13 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
+        <v>111</v>
+      </c>
+      <c r="C55" t="s">
         <v>112</v>
       </c>
-      <c r="C55" t="s">
-        <v>113</v>
-      </c>
       <c r="D55" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1835,13 +1835,13 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
+        <v>113</v>
+      </c>
+      <c r="C56" t="s">
         <v>114</v>
       </c>
-      <c r="C56" t="s">
-        <v>115</v>
-      </c>
       <c r="D56" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1849,13 +1849,13 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
+        <v>115</v>
+      </c>
+      <c r="C57" t="s">
         <v>116</v>
       </c>
-      <c r="C57" t="s">
-        <v>117</v>
-      </c>
       <c r="D57" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1863,13 +1863,13 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
+        <v>117</v>
+      </c>
+      <c r="C58" t="s">
         <v>118</v>
       </c>
-      <c r="C58" t="s">
-        <v>119</v>
-      </c>
       <c r="D58" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1877,13 +1877,13 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
+        <v>119</v>
+      </c>
+      <c r="C59" t="s">
         <v>120</v>
       </c>
-      <c r="C59" t="s">
-        <v>121</v>
-      </c>
       <c r="D59" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1891,13 +1891,13 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
+        <v>121</v>
+      </c>
+      <c r="C60" t="s">
         <v>122</v>
       </c>
-      <c r="C60" t="s">
-        <v>123</v>
-      </c>
       <c r="D60" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1905,13 +1905,13 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
+        <v>123</v>
+      </c>
+      <c r="C61" t="s">
         <v>124</v>
       </c>
-      <c r="C61" t="s">
-        <v>125</v>
-      </c>
       <c r="D61" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1919,13 +1919,13 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
+        <v>125</v>
+      </c>
+      <c r="C62" t="s">
         <v>126</v>
       </c>
-      <c r="C62" t="s">
-        <v>127</v>
-      </c>
       <c r="D62" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1933,13 +1933,13 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
+        <v>127</v>
+      </c>
+      <c r="C63" t="s">
         <v>128</v>
       </c>
-      <c r="C63" t="s">
-        <v>129</v>
-      </c>
       <c r="D63" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1947,13 +1947,13 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
+        <v>129</v>
+      </c>
+      <c r="C64" t="s">
         <v>130</v>
       </c>
-      <c r="C64" t="s">
-        <v>131</v>
-      </c>
       <c r="D64" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1961,13 +1961,13 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
+        <v>131</v>
+      </c>
+      <c r="C65" t="s">
         <v>132</v>
       </c>
-      <c r="C65" t="s">
-        <v>133</v>
-      </c>
       <c r="D65" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1975,13 +1975,13 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
+        <v>133</v>
+      </c>
+      <c r="C66" t="s">
         <v>134</v>
       </c>
-      <c r="C66" t="s">
-        <v>135</v>
-      </c>
       <c r="D66" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -1989,13 +1989,13 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
+        <v>135</v>
+      </c>
+      <c r="C67" t="s">
         <v>136</v>
       </c>
-      <c r="C67" t="s">
-        <v>137</v>
-      </c>
       <c r="D67" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -2003,13 +2003,13 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
+        <v>137</v>
+      </c>
+      <c r="C68" t="s">
         <v>138</v>
       </c>
-      <c r="C68" t="s">
-        <v>139</v>
-      </c>
       <c r="D68" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -2017,13 +2017,13 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
+        <v>139</v>
+      </c>
+      <c r="C69" t="s">
         <v>140</v>
       </c>
-      <c r="C69" t="s">
-        <v>141</v>
-      </c>
       <c r="D69" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -2031,13 +2031,13 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
+        <v>141</v>
+      </c>
+      <c r="C70" t="s">
         <v>142</v>
       </c>
-      <c r="C70" t="s">
-        <v>143</v>
-      </c>
       <c r="D70" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -2045,13 +2045,13 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
+        <v>143</v>
+      </c>
+      <c r="C71" t="s">
         <v>144</v>
       </c>
-      <c r="C71" t="s">
-        <v>145</v>
-      </c>
       <c r="D71" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -2059,13 +2059,13 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
+        <v>145</v>
+      </c>
+      <c r="C72" t="s">
         <v>146</v>
       </c>
-      <c r="C72" t="s">
-        <v>147</v>
-      </c>
       <c r="D72" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2073,13 +2073,13 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
+        <v>147</v>
+      </c>
+      <c r="C73" t="s">
         <v>148</v>
       </c>
-      <c r="C73" t="s">
-        <v>149</v>
-      </c>
       <c r="D73" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2087,13 +2087,13 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
+        <v>149</v>
+      </c>
+      <c r="C74" t="s">
         <v>150</v>
       </c>
-      <c r="C74" t="s">
-        <v>151</v>
-      </c>
       <c r="D74" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2101,13 +2101,13 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
+        <v>151</v>
+      </c>
+      <c r="C75" t="s">
         <v>152</v>
       </c>
-      <c r="C75" t="s">
-        <v>153</v>
-      </c>
       <c r="D75" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2115,13 +2115,13 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
+        <v>153</v>
+      </c>
+      <c r="C76" t="s">
         <v>154</v>
       </c>
-      <c r="C76" t="s">
-        <v>155</v>
-      </c>
       <c r="D76" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2129,13 +2129,13 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
+        <v>155</v>
+      </c>
+      <c r="C77" t="s">
         <v>156</v>
       </c>
-      <c r="C77" t="s">
-        <v>157</v>
-      </c>
       <c r="D77" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -2143,13 +2143,13 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
+        <v>157</v>
+      </c>
+      <c r="C78" t="s">
         <v>158</v>
       </c>
-      <c r="C78" t="s">
-        <v>159</v>
-      </c>
       <c r="D78" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -2157,13 +2157,13 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
+        <v>159</v>
+      </c>
+      <c r="C79" t="s">
         <v>160</v>
       </c>
-      <c r="C79" t="s">
-        <v>161</v>
-      </c>
       <c r="D79" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2171,13 +2171,13 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
+        <v>161</v>
+      </c>
+      <c r="C80" t="s">
         <v>162</v>
       </c>
-      <c r="C80" t="s">
-        <v>163</v>
-      </c>
       <c r="D80" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2185,13 +2185,13 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
+        <v>163</v>
+      </c>
+      <c r="C81" t="s">
         <v>164</v>
       </c>
-      <c r="C81" t="s">
-        <v>165</v>
-      </c>
       <c r="D81" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -2199,13 +2199,13 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
+        <v>165</v>
+      </c>
+      <c r="C82" t="s">
         <v>166</v>
       </c>
-      <c r="C82" t="s">
-        <v>167</v>
-      </c>
       <c r="D82" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2213,13 +2213,13 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
+        <v>167</v>
+      </c>
+      <c r="C83" t="s">
         <v>168</v>
       </c>
-      <c r="C83" t="s">
-        <v>169</v>
-      </c>
       <c r="D83" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2227,13 +2227,13 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
+        <v>169</v>
+      </c>
+      <c r="C84" t="s">
         <v>170</v>
       </c>
-      <c r="C84" t="s">
-        <v>171</v>
-      </c>
       <c r="D84" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2241,13 +2241,13 @@
         <v>84</v>
       </c>
       <c r="B85" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C85" t="s">
         <v>172</v>
       </c>
-      <c r="C85" t="s">
-        <v>173</v>
-      </c>
       <c r="D85" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -2255,13 +2255,13 @@
         <v>85</v>
       </c>
       <c r="B86" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C86" t="s">
         <v>174</v>
       </c>
-      <c r="C86" t="s">
-        <v>175</v>
-      </c>
       <c r="D86" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2269,13 +2269,13 @@
         <v>86</v>
       </c>
       <c r="B87" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C87" t="s">
         <v>176</v>
       </c>
-      <c r="C87" t="s">
-        <v>177</v>
-      </c>
       <c r="D87" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2283,13 +2283,13 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
+        <v>177</v>
+      </c>
+      <c r="C88" t="s">
         <v>178</v>
       </c>
-      <c r="C88" t="s">
-        <v>179</v>
-      </c>
       <c r="D88" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2297,13 +2297,13 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
+        <v>179</v>
+      </c>
+      <c r="C89" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="C89" s="12" t="s">
-        <v>181</v>
-      </c>
       <c r="D89" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -2311,13 +2311,13 @@
         <v>89</v>
       </c>
       <c r="B90" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C90" t="s">
         <v>182</v>
       </c>
-      <c r="C90" t="s">
-        <v>183</v>
-      </c>
       <c r="D90" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2342,7 +2342,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2351,218 +2351,218 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="10">
         <v>1</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="10">
         <v>2</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="10">
         <v>3</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="10">
         <v>4</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="10">
         <v>5</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="10">
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F16" s="11"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="10">
         <v>2</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="10">
         <v>3</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B19" s="10">
         <v>4</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" s="10">
         <v>5</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -2581,6 +2581,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -2821,18 +2833,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
   <ds:schemaRefs>
@@ -2842,6 +2842,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52DF9303-7267-4D15-A5CD-CFC88FA1FEC6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2858,21 +2875,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
GL-1 changes in DPE and DD for GINI and DPE for LISA
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_GINI_P1.xlsx
+++ b/rmonize/data_dictionary/DD_GINI_P1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBF8566-83AC-446A-97EF-862086C728ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3336BE2-AF4B-45D8-903B-1182C1C9CDED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="213">
   <si>
     <t>index</t>
   </si>
@@ -630,6 +630,42 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>aktivleiisommn_15</t>
+  </si>
+  <si>
+    <t>Number of hours in a normal week (7 days) with light physical activity of the child (without sweating, normal breathing, e.g. walking) in summer [hours]</t>
+  </si>
+  <si>
+    <t>aktivleiwintn_15</t>
+  </si>
+  <si>
+    <t>Number of hours in a normal week (7 days) with light physical activity of the child (without sweating, normal breathing, e.g. walking) in winter [hours]</t>
+  </si>
+  <si>
+    <t>aktivmitsommn_15</t>
+  </si>
+  <si>
+    <t>Number of hours in a normal week (7 days) with moderate physical activity (a little sweating, slightly increased breathing e.g. cycling, swimming, skating) in summer [hours]</t>
+  </si>
+  <si>
+    <t>aktivmitwintn_15</t>
+  </si>
+  <si>
+    <t>Number of hours in a normal week (7 days) with moderate physical activity (some sweating, slightly increased breathing e.g. cycling, swimming, skating) in winter [hours]</t>
+  </si>
+  <si>
+    <t>aktivschsommn_15</t>
+  </si>
+  <si>
+    <t>Number of hours in a normal week (7 days) with heavy physical activity (a lot of sweating, rapid breathing, e.g. ball games, training) in summer [hours]</t>
+  </si>
+  <si>
+    <t>aktivschwintn_15</t>
+  </si>
+  <si>
+    <t>Number of hours in a normal week (7 days) with heavy physical activity (a lot of sweating, rapid breathing, e.g. ball games, training) in winter [hours]</t>
   </si>
 </sst>
 </file>
@@ -1047,20 +1083,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A73012-5CAD-43B9-A281-79101DF4E1E0}">
-  <dimension ref="A1:D90"/>
+  <dimension ref="A1:D96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2:A96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="53.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125"/>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="3" max="3" width="53.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1074,7 +1110,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1088,7 +1124,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1102,7 +1138,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1116,7 +1152,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1130,7 +1166,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1144,1179 +1180,1263 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C7" t="s">
+        <v>202</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>203</v>
+      </c>
+      <c r="C8" t="s">
+        <v>204</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>205</v>
+      </c>
+      <c r="C9" t="s">
+        <v>206</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>21</v>
+      <c r="B10" t="s">
+        <v>207</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>208</v>
       </c>
       <c r="D10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>23</v>
+      <c r="B11" t="s">
+        <v>209</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>210</v>
       </c>
       <c r="D11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>25</v>
+      <c r="B12" t="s">
+        <v>211</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>212</v>
       </c>
       <c r="D12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>33</v>
+      <c r="B16" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>35</v>
+      <c r="B17" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D24" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D25" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C26" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>56</v>
+        <v>43</v>
+      </c>
+      <c r="C27" t="s">
+        <v>44</v>
       </c>
       <c r="D27" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C28" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="D28" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D29" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C30" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D30" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
-        <v>63</v>
+      <c r="B31" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="C31" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D31" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" t="s">
-        <v>65</v>
+      <c r="B32" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="C32" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D32" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" t="s">
-        <v>67</v>
-      </c>
-      <c r="C33" t="s">
-        <v>68</v>
+      <c r="B33" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="D33" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" t="s">
-        <v>69</v>
+      <c r="B34" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="C34" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="D34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" t="s">
-        <v>71</v>
+      <c r="B35" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="C35" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="D35" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" t="s">
-        <v>73</v>
+      <c r="B36" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="C36" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="D36" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C37" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="D37" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C38" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D38" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="C39" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="D39" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C40" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="D40" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>83</v>
-      </c>
-      <c r="C41" s="13" t="s">
-        <v>84</v>
+        <v>71</v>
+      </c>
+      <c r="C41" t="s">
+        <v>72</v>
       </c>
       <c r="D41" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="C42" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="D42" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="C43" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="D43" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="C44" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="D44" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="C45" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="D45" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="C46" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="D46" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>95</v>
-      </c>
-      <c r="C47" t="s">
-        <v>96</v>
+        <v>83</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>84</v>
       </c>
       <c r="D47" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="C48" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="D48" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
-      <c r="B49" s="3" t="s">
-        <v>99</v>
+      <c r="B49" t="s">
+        <v>87</v>
       </c>
       <c r="C49" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="D49" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="C50" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="D50" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="C51" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="D51" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="C52" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="D52" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C53" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="D53" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="C54" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="D54" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
-      <c r="B55" t="s">
-        <v>111</v>
+      <c r="B55" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="C55" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="D55" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="C56" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="D56" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="C57" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="D57" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="C58" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="D58" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="C59" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="D59" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="C60" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="D60" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="C61" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="D61" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="C62" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="D62" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="C63" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="D63" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="C64" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="D64" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="C65" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="D65" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="C66" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="D66" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="C67" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="D67" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="C68" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="D68" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C69" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D69" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="C70" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="D70" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="C71" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="D71" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="C72" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="D72" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="C73" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="D73" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="C74" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="D74" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="C75" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="D75" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="C76" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="D76" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="C77" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="D77" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C78" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="D78" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C79" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="D79" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="C80" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="D80" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="C81" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="D81" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="C82" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="D82" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="C83" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="D83" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="C84" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="D84" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
-      <c r="B85" s="3" t="s">
-        <v>171</v>
+      <c r="B85" t="s">
+        <v>159</v>
       </c>
       <c r="C85" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="D85" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
-      <c r="B86" s="3" t="s">
-        <v>173</v>
+      <c r="B86" t="s">
+        <v>161</v>
       </c>
       <c r="C86" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="D86" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
-      <c r="B87" s="3" t="s">
-        <v>175</v>
+      <c r="B87" t="s">
+        <v>163</v>
       </c>
       <c r="C87" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="D87" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="C88" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="D88" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>179</v>
-      </c>
-      <c r="C89" s="12" t="s">
-        <v>180</v>
+        <v>167</v>
+      </c>
+      <c r="C89" t="s">
+        <v>168</v>
       </c>
       <c r="D89" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B90" t="s">
+        <v>169</v>
+      </c>
+      <c r="C90" t="s">
+        <v>170</v>
+      </c>
+      <c r="D90" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C91" t="s">
+        <v>172</v>
+      </c>
+      <c r="D91" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C92" t="s">
+        <v>174</v>
+      </c>
+      <c r="D92" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C93" t="s">
+        <v>176</v>
+      </c>
+      <c r="D93" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>177</v>
+      </c>
+      <c r="C94" t="s">
+        <v>178</v>
+      </c>
+      <c r="D94" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>179</v>
+      </c>
+      <c r="C95" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="D95" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C96" t="s">
         <v>182</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D96" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2334,13 +2454,13 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>183</v>
       </c>
@@ -2355,7 +2475,7 @@
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2366,7 +2486,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -2377,7 +2497,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
@@ -2388,7 +2508,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -2399,7 +2519,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -2410,7 +2530,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
@@ -2421,7 +2541,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -2432,7 +2552,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
@@ -2443,7 +2563,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2454,7 +2574,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -2465,7 +2585,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2476,7 +2596,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2487,7 +2607,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -2498,7 +2618,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -2509,7 +2629,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -2521,7 +2641,7 @@
       </c>
       <c r="F16" s="11"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -2532,7 +2652,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -2543,7 +2663,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -2554,7 +2674,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -2572,15 +2692,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
@@ -2590,6 +2701,15 @@
     <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2834,14 +2954,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2854,6 +2966,14 @@
     <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
GL-4 DD_GINI_P1 small change to keep consistent with P2
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_GINI_P1.xlsx
+++ b/rmonize/data_dictionary/DD_GINI_P1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\rmonize\data_dictionary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3336BE2-AF4B-45D8-903B-1182C1C9CDED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E3838A-CD85-47E3-AEB3-41F2C7F662EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="22290" windowHeight="12000" activeTab="1" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="212">
   <si>
     <t>index</t>
   </si>
@@ -603,9 +603,6 @@
   </si>
   <si>
     <t>Sonstiger Abschluss</t>
-  </si>
-  <si>
-    <t>kein Abschluss</t>
   </si>
   <si>
     <t>Hochschule/Fachhochschuli/Universität</t>
@@ -771,7 +768,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -787,9 +784,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -827,7 +824,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -933,7 +930,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1075,7 +1072,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1085,18 +1082,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A73012-5CAD-43B9-A281-79101DF4E1E0}">
   <dimension ref="A1:D96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.109375" customWidth="1"/>
-    <col min="3" max="3" width="53.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="53.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1110,12 +1107,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>4</v>
@@ -1124,7 +1121,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1138,7 +1135,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1152,7 +1149,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1166,7 +1163,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1180,91 +1177,91 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C7" t="s">
         <v>201</v>
       </c>
-      <c r="C7" t="s">
-        <v>202</v>
-      </c>
       <c r="D7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>202</v>
+      </c>
+      <c r="C8" t="s">
         <v>203</v>
       </c>
-      <c r="C8" t="s">
-        <v>204</v>
-      </c>
       <c r="D8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>204</v>
+      </c>
+      <c r="C9" t="s">
         <v>205</v>
       </c>
-      <c r="C9" t="s">
-        <v>206</v>
-      </c>
       <c r="D9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C10" t="s">
         <v>207</v>
       </c>
-      <c r="C10" t="s">
-        <v>208</v>
-      </c>
       <c r="D10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>208</v>
+      </c>
+      <c r="C11" t="s">
         <v>209</v>
       </c>
-      <c r="C11" t="s">
-        <v>210</v>
-      </c>
       <c r="D11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>210</v>
+      </c>
+      <c r="C12" t="s">
         <v>211</v>
       </c>
-      <c r="C12" t="s">
-        <v>212</v>
-      </c>
       <c r="D12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1278,7 +1275,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1292,7 +1289,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1306,7 +1303,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1320,7 +1317,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1334,7 +1331,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1348,7 +1345,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1362,7 +1359,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1376,7 +1373,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1390,7 +1387,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1404,7 +1401,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1418,7 +1415,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1432,7 +1429,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1446,7 +1443,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1460,7 +1457,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1474,7 +1471,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1488,7 +1485,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1502,7 +1499,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1516,7 +1513,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1530,7 +1527,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1544,7 +1541,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1558,7 +1555,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1572,7 +1569,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1586,7 +1583,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1600,7 +1597,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1614,7 +1611,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1628,7 +1625,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1642,7 +1639,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1656,7 +1653,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1670,7 +1667,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1684,7 +1681,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1698,7 +1695,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1712,7 +1709,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1726,7 +1723,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1740,7 +1737,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1754,7 +1751,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1768,7 +1765,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1782,7 +1779,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1796,7 +1793,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1810,7 +1807,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1824,7 +1821,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1838,7 +1835,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1852,7 +1849,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1866,7 +1863,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1880,7 +1877,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1894,7 +1891,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1908,7 +1905,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1922,7 +1919,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1936,7 +1933,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1950,7 +1947,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1964,7 +1961,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1978,7 +1975,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1992,7 +1989,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2006,7 +2003,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2020,7 +2017,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2034,7 +2031,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2048,7 +2045,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2062,7 +2059,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2076,7 +2073,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2090,7 +2087,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2104,7 +2101,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2118,7 +2115,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2132,7 +2129,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2146,7 +2143,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2160,7 +2157,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2174,7 +2171,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2188,7 +2185,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2202,7 +2199,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2216,7 +2213,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2230,7 +2227,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2244,7 +2241,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2258,7 +2255,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2272,7 +2269,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2286,7 +2283,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2300,7 +2297,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2314,7 +2311,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2328,7 +2325,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2342,7 +2339,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2356,7 +2353,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2370,7 +2367,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2384,7 +2381,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2398,7 +2395,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -2412,7 +2409,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2426,7 +2423,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -2450,17 +2447,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7CFBFAA-22DC-428C-A718-7E0BADD40216}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>183</v>
       </c>
@@ -2475,7 +2472,7 @@
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2486,7 +2483,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -2497,7 +2494,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
@@ -2508,7 +2505,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -2519,7 +2516,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -2530,7 +2527,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
@@ -2541,7 +2538,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -2552,7 +2549,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
@@ -2560,10 +2557,10 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2574,7 +2571,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -2585,7 +2582,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2596,7 +2593,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2604,10 +2601,10 @@
         <v>4</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -2618,7 +2615,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -2626,10 +2623,10 @@
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -2637,11 +2634,11 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F16" s="11"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -2649,10 +2646,10 @@
         <v>2</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -2660,10 +2657,10 @@
         <v>3</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -2671,10 +2668,10 @@
         <v>4</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -2682,7 +2679,7 @@
         <v>5</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -2692,6 +2689,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
@@ -2701,15 +2707,6 @@
     <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2954,6 +2951,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2966,14 +2971,6 @@
     <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
GL-5 change in DD Education Variable
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_GINI_P1.xlsx
+++ b/rmonize/data_dictionary/DD_GINI_P1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_dictionary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E3838A-CD85-47E3-AEB3-41F2C7F662EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FF99F4-00C5-4937-A20C-D9E2912378C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="22290" windowHeight="12000" activeTab="1" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="224">
   <si>
     <t>index</t>
   </si>
@@ -663,6 +663,42 @@
   </si>
   <si>
     <t>Number of hours in a normal week (7 days) with heavy physical activity (a lot of sweating, rapid breathing, e.g. ball games, training) in winter [hours]</t>
+  </si>
+  <si>
+    <t>MUTBERU_3</t>
+  </si>
+  <si>
+    <t>VATBERU_3</t>
+  </si>
+  <si>
+    <t>Auszubildende/r, Student/in</t>
+  </si>
+  <si>
+    <t>kein beruflicher Abschluss</t>
+  </si>
+  <si>
+    <t>abgeschlossene beruflich-betriebliche Ausbildung</t>
+  </si>
+  <si>
+    <t>abgeschlossene beruflich-schulische Ausbildung</t>
+  </si>
+  <si>
+    <t>abgeschlossene Ausbildung an Fachschule</t>
+  </si>
+  <si>
+    <t>Fachhochschulabschluss</t>
+  </si>
+  <si>
+    <t>Hochschulabschluss</t>
+  </si>
+  <si>
+    <t>anderer beruflicher Abschluss</t>
+  </si>
+  <si>
+    <t>highest job qualification of the mother</t>
+  </si>
+  <si>
+    <t>highest job qualification of the father</t>
   </si>
 </sst>
 </file>
@@ -731,7 +767,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -766,9 +802,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -784,9 +823,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -824,7 +863,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -930,7 +969,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1072,7 +1111,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1080,13 +1119,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A73012-5CAD-43B9-A281-79101DF4E1E0}">
-  <dimension ref="A1:D96"/>
+  <dimension ref="A1:D98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A96"/>
+      <selection activeCell="A2" sqref="A2:A98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
     <col min="3" max="3" width="53.42578125" bestFit="1" customWidth="1"/>
@@ -1182,13 +1221,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="C7" t="s">
-        <v>201</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
+        <v>222</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1196,13 +1235,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>202</v>
-      </c>
-      <c r="C8" t="s">
-        <v>203</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
+        <v>213</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1210,10 +1249,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C9" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D9" t="s">
         <v>18</v>
@@ -1224,10 +1263,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C10" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D10" t="s">
         <v>18</v>
@@ -1238,10 +1277,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C11" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D11" t="s">
         <v>18</v>
@@ -1252,10 +1291,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C12" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D12" t="s">
         <v>18</v>
@@ -1265,27 +1304,27 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>5</v>
+      <c r="B13" t="s">
+        <v>208</v>
+      </c>
+      <c r="C13" t="s">
+        <v>209</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="6" t="s">
+      <c r="B14" t="s">
+        <v>210</v>
+      </c>
+      <c r="C14" t="s">
+        <v>211</v>
+      </c>
+      <c r="D14" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1293,27 +1332,27 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>18</v>
+      <c r="B15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="B16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1321,13 +1360,13 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="B17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1335,11 +1374,11 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>25</v>
+      <c r="B18" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D18" t="s">
         <v>18</v>
@@ -1349,11 +1388,11 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>27</v>
+      <c r="B19" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D19" t="s">
         <v>18</v>
@@ -1364,10 +1403,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D20" t="s">
         <v>18</v>
@@ -1378,10 +1417,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C21" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D21" t="s">
         <v>18</v>
@@ -1392,10 +1431,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D22" t="s">
         <v>18</v>
@@ -1406,10 +1445,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C23" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D23" t="s">
         <v>18</v>
@@ -1420,10 +1459,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D24" t="s">
         <v>18</v>
@@ -1434,10 +1473,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D25" t="s">
         <v>18</v>
@@ -1448,10 +1487,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C26" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D26" t="s">
         <v>18</v>
@@ -1462,10 +1501,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C27" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D27" t="s">
         <v>18</v>
@@ -1476,10 +1515,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C28" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D28" t="s">
         <v>18</v>
@@ -1490,10 +1529,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D29" t="s">
         <v>18</v>
@@ -1504,10 +1543,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C30" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D30" t="s">
         <v>18</v>
@@ -1518,10 +1557,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C31" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D31" t="s">
         <v>18</v>
@@ -1532,10 +1571,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C32" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D32" t="s">
         <v>18</v>
@@ -1546,10 +1585,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
+      </c>
+      <c r="C33" t="s">
+        <v>52</v>
       </c>
       <c r="D33" t="s">
         <v>18</v>
@@ -1560,10 +1599,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C34" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D34" t="s">
         <v>18</v>
@@ -1574,10 +1613,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C35" t="s">
-        <v>60</v>
+        <v>55</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="D35" t="s">
         <v>18</v>
@@ -1588,10 +1627,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C36" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D36" t="s">
         <v>18</v>
@@ -1601,11 +1640,11 @@
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" t="s">
-        <v>63</v>
+      <c r="B37" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="C37" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D37" t="s">
         <v>18</v>
@@ -1615,11 +1654,11 @@
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" t="s">
-        <v>65</v>
+      <c r="B38" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="C38" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D38" t="s">
         <v>18</v>
@@ -1630,10 +1669,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C39" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D39" t="s">
         <v>18</v>
@@ -1644,10 +1683,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C40" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D40" t="s">
         <v>18</v>
@@ -1658,10 +1697,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C41" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D41" t="s">
         <v>18</v>
@@ -1672,10 +1711,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C42" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D42" t="s">
         <v>18</v>
@@ -1686,10 +1725,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C43" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D43" t="s">
         <v>18</v>
@@ -1700,10 +1739,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C44" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D44" t="s">
         <v>18</v>
@@ -1714,10 +1753,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C45" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D45" t="s">
         <v>18</v>
@@ -1728,10 +1767,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C46" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D46" t="s">
         <v>18</v>
@@ -1742,10 +1781,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>83</v>
-      </c>
-      <c r="C47" s="13" t="s">
-        <v>84</v>
+        <v>79</v>
+      </c>
+      <c r="C47" t="s">
+        <v>80</v>
       </c>
       <c r="D47" t="s">
         <v>18</v>
@@ -1756,10 +1795,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C48" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D48" t="s">
         <v>18</v>
@@ -1770,10 +1809,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>87</v>
-      </c>
-      <c r="C49" t="s">
-        <v>88</v>
+        <v>83</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>84</v>
       </c>
       <c r="D49" t="s">
         <v>18</v>
@@ -1784,10 +1823,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C50" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D50" t="s">
         <v>18</v>
@@ -1798,10 +1837,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C51" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D51" t="s">
         <v>18</v>
@@ -1812,10 +1851,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C52" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D52" t="s">
         <v>18</v>
@@ -1826,10 +1865,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C53" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D53" t="s">
         <v>18</v>
@@ -1840,10 +1879,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C54" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D54" t="s">
         <v>18</v>
@@ -1853,11 +1892,11 @@
       <c r="A55">
         <v>54</v>
       </c>
-      <c r="B55" s="3" t="s">
-        <v>99</v>
+      <c r="B55" t="s">
+        <v>95</v>
       </c>
       <c r="C55" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D55" t="s">
         <v>18</v>
@@ -1868,10 +1907,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C56" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D56" t="s">
         <v>18</v>
@@ -1881,11 +1920,11 @@
       <c r="A57">
         <v>56</v>
       </c>
-      <c r="B57" t="s">
-        <v>103</v>
+      <c r="B57" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="C57" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D57" t="s">
         <v>18</v>
@@ -1896,10 +1935,10 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C58" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D58" t="s">
         <v>18</v>
@@ -1910,10 +1949,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C59" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D59" t="s">
         <v>18</v>
@@ -1924,10 +1963,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C60" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D60" t="s">
         <v>18</v>
@@ -1938,10 +1977,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C61" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D61" t="s">
         <v>18</v>
@@ -1952,10 +1991,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C62" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D62" t="s">
         <v>18</v>
@@ -1966,10 +2005,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C63" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D63" t="s">
         <v>18</v>
@@ -1980,10 +2019,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C64" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D64" t="s">
         <v>18</v>
@@ -1994,10 +2033,10 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C65" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D65" t="s">
         <v>18</v>
@@ -2008,10 +2047,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C66" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D66" t="s">
         <v>18</v>
@@ -2022,10 +2061,10 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C67" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D67" t="s">
         <v>18</v>
@@ -2036,10 +2075,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C68" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D68" t="s">
         <v>18</v>
@@ -2050,10 +2089,10 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C69" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D69" t="s">
         <v>18</v>
@@ -2064,10 +2103,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C70" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D70" t="s">
         <v>18</v>
@@ -2078,10 +2117,10 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C71" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D71" t="s">
         <v>18</v>
@@ -2092,10 +2131,10 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C72" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D72" t="s">
         <v>18</v>
@@ -2106,10 +2145,10 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C73" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D73" t="s">
         <v>18</v>
@@ -2120,10 +2159,10 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C74" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D74" t="s">
         <v>18</v>
@@ -2134,10 +2173,10 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C75" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D75" t="s">
         <v>18</v>
@@ -2148,10 +2187,10 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C76" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D76" t="s">
         <v>18</v>
@@ -2162,10 +2201,10 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C77" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D77" t="s">
         <v>18</v>
@@ -2176,10 +2215,10 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C78" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D78" t="s">
         <v>18</v>
@@ -2190,10 +2229,10 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C79" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D79" t="s">
         <v>18</v>
@@ -2204,10 +2243,10 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C80" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D80" t="s">
         <v>18</v>
@@ -2218,10 +2257,10 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C81" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D81" t="s">
         <v>18</v>
@@ -2232,10 +2271,10 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C82" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D82" t="s">
         <v>18</v>
@@ -2246,10 +2285,10 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C83" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D83" t="s">
         <v>18</v>
@@ -2260,10 +2299,10 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C84" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D84" t="s">
         <v>18</v>
@@ -2274,10 +2313,10 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C85" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D85" t="s">
         <v>18</v>
@@ -2288,10 +2327,10 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C86" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D86" t="s">
         <v>18</v>
@@ -2302,10 +2341,10 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C87" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D87" t="s">
         <v>18</v>
@@ -2316,10 +2355,10 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C88" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D88" t="s">
         <v>18</v>
@@ -2330,10 +2369,10 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C89" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D89" t="s">
         <v>18</v>
@@ -2344,10 +2383,10 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C90" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D90" t="s">
         <v>18</v>
@@ -2357,11 +2396,11 @@
       <c r="A91">
         <v>90</v>
       </c>
-      <c r="B91" s="3" t="s">
-        <v>171</v>
+      <c r="B91" t="s">
+        <v>167</v>
       </c>
       <c r="C91" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D91" t="s">
         <v>18</v>
@@ -2371,11 +2410,11 @@
       <c r="A92">
         <v>91</v>
       </c>
-      <c r="B92" s="3" t="s">
-        <v>173</v>
+      <c r="B92" t="s">
+        <v>169</v>
       </c>
       <c r="C92" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D92" t="s">
         <v>18</v>
@@ -2386,10 +2425,10 @@
         <v>92</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C93" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D93" t="s">
         <v>18</v>
@@ -2399,11 +2438,11 @@
       <c r="A94">
         <v>93</v>
       </c>
-      <c r="B94" t="s">
-        <v>177</v>
+      <c r="B94" s="3" t="s">
+        <v>173</v>
       </c>
       <c r="C94" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D94" t="s">
         <v>18</v>
@@ -2413,11 +2452,11 @@
       <c r="A95">
         <v>94</v>
       </c>
-      <c r="B95" t="s">
-        <v>179</v>
-      </c>
-      <c r="C95" s="12" t="s">
-        <v>180</v>
+      <c r="B95" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C95" t="s">
+        <v>176</v>
       </c>
       <c r="D95" t="s">
         <v>18</v>
@@ -2427,13 +2466,41 @@
       <c r="A96">
         <v>95</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="B96" t="s">
+        <v>177</v>
+      </c>
+      <c r="C96" t="s">
+        <v>178</v>
+      </c>
+      <c r="D96" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>179</v>
+      </c>
+      <c r="C97" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="D97" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C98" t="s">
         <v>182</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D98" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2445,13 +2512,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7CFBFAA-22DC-428C-A718-7E0BADD40216}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50.85546875" bestFit="1" customWidth="1"/>
@@ -2682,6 +2749,182 @@
         <v>198</v>
       </c>
     </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>212</v>
+      </c>
+      <c r="B21" s="10">
+        <v>1</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>212</v>
+      </c>
+      <c r="B22" s="10">
+        <v>2</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>212</v>
+      </c>
+      <c r="B23" s="10">
+        <v>3</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>212</v>
+      </c>
+      <c r="B24" s="10">
+        <v>4</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>212</v>
+      </c>
+      <c r="B25" s="10">
+        <v>5</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>212</v>
+      </c>
+      <c r="B26" s="10">
+        <v>6</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>212</v>
+      </c>
+      <c r="B27" s="10">
+        <v>7</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>212</v>
+      </c>
+      <c r="B28" s="10">
+        <v>8</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>213</v>
+      </c>
+      <c r="B29" s="10">
+        <v>1</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>213</v>
+      </c>
+      <c r="B30" s="10">
+        <v>2</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>213</v>
+      </c>
+      <c r="B31" s="10">
+        <v>3</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>213</v>
+      </c>
+      <c r="B32" s="10">
+        <v>4</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>213</v>
+      </c>
+      <c r="B33" s="10">
+        <v>5</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>213</v>
+      </c>
+      <c r="B34" s="10">
+        <v>6</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>213</v>
+      </c>
+      <c r="B35" s="10">
+        <v>7</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>213</v>
+      </c>
+      <c r="B36" s="10">
+        <v>8</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>221</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2689,15 +2932,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
@@ -2707,6 +2941,15 @@
     <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2951,14 +3194,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2971,6 +3206,14 @@
     <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>